<commit_message>
atualização requisitos e backlog
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/backlog.xlsx
+++ b/Documentação/Backlog/backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Desktop\Mind6\Mind6\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cicer\Desktop\Mind6\Mind6\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EBC57A-846B-43DC-8BCF-F2614518FD4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92852B8E-B803-474C-BADF-DC95742F7F07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
   <si>
     <t>Essencial</t>
   </si>
@@ -193,6 +193,27 @@
   </si>
   <si>
     <t>César</t>
+  </si>
+  <si>
+    <t>executáve(jar)</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>dashboard estático</t>
+  </si>
+  <si>
+    <t>médio</t>
+  </si>
+  <si>
+    <t>Não iniciado</t>
+  </si>
+  <si>
+    <t>todos</t>
+  </si>
+  <si>
+    <t>vicari,cardoso,cesar</t>
   </si>
 </sst>
 </file>
@@ -351,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -417,11 +438,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -442,63 +526,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -646,8 +673,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{790BF426-3166-4ADE-AA13-1E47202751F1}" name="Tabela9" displayName="Tabela9" ref="I3:L21" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="I3:L21" xr:uid="{88EC5994-83AA-49C2-95D5-5D462715856F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{790BF426-3166-4ADE-AA13-1E47202751F1}" name="Tabela9" displayName="Tabela9" ref="I3:L23" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="I3:L23" xr:uid="{88EC5994-83AA-49C2-95D5-5D462715856F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -664,7 +691,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A9C2F173-C49B-42FE-AD89-B41469A1A209}" name="Tabela11" displayName="Tabela11" ref="B2:F17" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A9C2F173-C49B-42FE-AD89-B41469A1A209}" name="Tabela11" displayName="Tabela11" ref="B2:F17" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="B2:F17" xr:uid="{59808F07-3281-4454-A044-686B6C49FAEA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -673,11 +700,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{919E5654-60D8-47A9-9ADF-1483731E1AFD}" name="BackLog" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{A68969C8-98EE-4A0A-969E-F57A1E39322B}" name="Classificação" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{208B8D16-0364-498D-9399-9884BE0F1BA4}" name="Prioridade" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{C9A670FA-54D8-4A99-B56B-614FC1239D9E}" name="Funcional/Não Funcional" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{D53AC345-E337-4799-ADC3-8693459DF325}" name="Dificuldade" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{919E5654-60D8-47A9-9ADF-1483731E1AFD}" name="BackLog" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A68969C8-98EE-4A0A-969E-F57A1E39322B}" name="Classificação" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{208B8D16-0364-498D-9399-9884BE0F1BA4}" name="Prioridade" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C9A670FA-54D8-4A99-B56B-614FC1239D9E}" name="Funcional/Não Funcional" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D53AC345-E337-4799-ADC3-8693459DF325}" name="Dificuldade" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -946,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA74D22E-D97A-4A36-8A23-C71CA6BE156D}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,6 +1508,34 @@
         <v>39</v>
       </c>
     </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I22" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I23" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
mudanças na documentaçãoe  no ppt
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/backlog.xlsx
+++ b/Documentação/Backlog/backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Desktop\Mind6\Mind6\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cicer\Desktop\Mind6\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72498082-5011-4FDD-9D44-11D3444B1845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FE1FD0-89C2-4668-875C-024EF2509671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,18 +51,12 @@
     <t>Página Web de Login</t>
   </si>
   <si>
-    <t>Ferramenta de HelpDesk</t>
-  </si>
-  <si>
     <t>Banco de Dados na Nuvem</t>
   </si>
   <si>
     <t>Gerar relatórios</t>
   </si>
   <si>
-    <t>Enviar mensagens via Telegram</t>
-  </si>
-  <si>
     <t>Avisos de erros</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>Utilizar a API OSHI</t>
+  </si>
+  <si>
+    <t>Enviar mensagens via Slack</t>
+  </si>
+  <si>
+    <t>Ferramenta de HelpDesk(Tom ticket)</t>
   </si>
 </sst>
 </file>
@@ -368,9 +368,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,6 +415,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,7 +950,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,46 +973,46 @@
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="I1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="17" t="s">
+      <c r="I1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="J2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1023,25 +1023,25 @@
         <v>0</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4">
         <v>21</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>30</v>
+      <c r="I3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1052,25 +1052,25 @@
         <v>0</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" s="4">
         <v>13</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>30</v>
+      <c r="I4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1081,54 +1081,54 @@
         <v>0</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F5" s="4">
         <v>8</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="12" t="s">
+      <c r="I5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>38</v>
+      <c r="B6" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>31</v>
+      <c r="I6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1139,25 +1139,25 @@
         <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7" s="4">
         <v>5</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="13" t="s">
+      <c r="I7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>30</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1168,25 +1168,25 @@
         <v>0</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>31</v>
+      <c r="I8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1197,319 +1197,319 @@
         <v>0</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F9" s="4">
         <v>5</v>
       </c>
-      <c r="I9" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>49</v>
+      <c r="I9" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="4">
         <v>8</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>30</v>
+      <c r="I10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F11" s="4">
         <v>5</v>
       </c>
-      <c r="I11" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>30</v>
+      <c r="I11" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" s="4">
         <v>21</v>
       </c>
-      <c r="I12" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>30</v>
+      <c r="I12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F13" s="4">
         <v>13</v>
       </c>
-      <c r="I13" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>30</v>
+      <c r="I13" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="4">
         <v>8</v>
       </c>
-      <c r="I14" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>30</v>
+      <c r="I14" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" s="4">
         <v>21</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>30</v>
+      <c r="I15" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" s="4">
         <v>8</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>30</v>
+      <c r="I16" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="F17" s="4">
         <v>21</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="26"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>37</v>
+      <c r="D18" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="F18" s="4">
         <v>21</v>
       </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="26"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="26"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="25"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I20" s="24"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="26"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I21" s="24"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="26"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="26"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="25"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I23" s="24"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="26"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="25"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I24" s="24"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="25"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I25" s="24"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="25"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I26" s="24"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="26"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>